<commit_message>
plotting gtruth from pipeline
</commit_message>
<xml_diff>
--- a/pipeline/cell_type_mapping.xlsx
+++ b/pipeline/cell_type_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D7889B-1BA6-4E86-A375-E51B87ED65E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FFCD9F-BA25-4D63-BB4F-464A893914EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="294">
   <si>
     <t>cell_type</t>
   </si>
@@ -882,9 +882,6 @@
   </si>
   <si>
     <t>mDC</t>
-  </si>
-  <si>
-    <t>myeloid dendritic cell</t>
   </si>
   <si>
     <t>vanderbilt_lung</t>
@@ -3197,8 +3194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B233" sqref="B233"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C272" sqref="C272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -6311,7 +6308,7 @@
         <v>224</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>17</v>
@@ -6325,7 +6322,7 @@
         <v>224</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>17</v>
@@ -6395,7 +6392,7 @@
         <v>224</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>17</v>
@@ -6505,7 +6502,7 @@
         <v>244</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>252</v>
@@ -6565,7 +6562,7 @@
         <v>244</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C237" s="5" t="s">
         <v>252</v>
@@ -6579,7 +6576,7 @@
         <v>244</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>252</v>
@@ -6773,7 +6770,7 @@
         <v>244</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>262</v>
@@ -6806,7 +6803,7 @@
         <v>244</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>17</v>
@@ -6817,7 +6814,7 @@
         <v>244</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>17</v>
@@ -6916,7 +6913,7 @@
         <v>244</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>17</v>
@@ -7018,7 +7015,7 @@
         <v>281</v>
       </c>
       <c r="C274" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -7078,10 +7075,10 @@
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B280" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="B280" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="C280" t="s">
         <v>54</v>
@@ -7089,10 +7086,10 @@
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C281" t="s">
         <v>53</v>
@@ -7100,10 +7097,10 @@
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C282" t="s">
         <v>54</v>
@@ -7111,10 +7108,10 @@
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C283" t="s">
         <v>53</v>
@@ -7122,10 +7119,10 @@
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B284" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="B284" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="C284" t="s">
         <v>61</v>

</xml_diff>